<commit_message>
Remove unused && freeze first column
</commit_message>
<xml_diff>
--- a/marneus_calgar.xlsx
+++ b/marneus_calgar.xlsx
@@ -946,8 +946,10 @@
   <dimension ref="A1:L181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>